<commit_message>
Add mediapipe to Object RealTime Detection
</commit_message>
<xml_diff>
--- a/FaceWebApp/ObjectDetected.xlsx
+++ b/FaceWebApp/ObjectDetected.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B201"/>
+  <dimension ref="A1:B435"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,7 +439,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>60.93</v>
+        <v>85.20999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -449,7 +449,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>68.3</v>
+        <v>65.44</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>64.83</v>
+        <v>63.73</v>
       </c>
     </row>
     <row r="5">
@@ -469,27 +469,27 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>66.42</v>
+        <v>52.05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>68.87</v>
+        <v>51.42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Bench</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>68.91</v>
+        <v>50.47</v>
       </c>
     </row>
     <row r="8">
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>69.12</v>
+        <v>86.02</v>
       </c>
     </row>
     <row r="9">
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>69.65000000000001</v>
+        <v>69.09</v>
       </c>
     </row>
     <row r="10">
@@ -519,37 +519,37 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>70.56</v>
+        <v>66.27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Bench</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>68.08</v>
+        <v>52.65</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>65.98</v>
+        <v>52.33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Bottle</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>51.59</v>
+        <v>85.7</v>
       </c>
     </row>
     <row r="14">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>65.25</v>
+        <v>70.40000000000001</v>
       </c>
     </row>
     <row r="15">
@@ -569,17 +569,17 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>53.94</v>
+        <v>62.26</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>65.23</v>
+        <v>53.22</v>
       </c>
     </row>
     <row r="17">
@@ -589,7 +589,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>57.72</v>
+        <v>86.77</v>
       </c>
     </row>
     <row r="18">
@@ -599,7 +599,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>65.02</v>
+        <v>70.73</v>
       </c>
     </row>
     <row r="19">
@@ -609,17 +609,17 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>53.92</v>
+        <v>60.83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>64.41</v>
+        <v>52.53</v>
       </c>
     </row>
     <row r="21">
@@ -629,7 +629,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>62.04</v>
+        <v>84.55</v>
       </c>
     </row>
     <row r="22">
@@ -639,7 +639,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>65.90000000000001</v>
+        <v>70.68000000000001</v>
       </c>
     </row>
     <row r="23">
@@ -649,17 +649,17 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>64.95999999999999</v>
+        <v>59.28</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>64.81</v>
+        <v>55.54</v>
       </c>
     </row>
     <row r="25">
@@ -669,7 +669,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>63.85</v>
+        <v>71.06</v>
       </c>
     </row>
     <row r="26">
@@ -679,17 +679,17 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>64.44</v>
+        <v>69.59999999999999</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>58.01</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28">
@@ -699,7 +699,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>66.12</v>
+        <v>55.02</v>
       </c>
     </row>
     <row r="29">
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>65.64</v>
+        <v>70.95</v>
       </c>
     </row>
     <row r="30">
@@ -719,7 +719,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>65.66</v>
+        <v>61.89</v>
       </c>
     </row>
     <row r="31">
@@ -729,27 +729,27 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>66.36</v>
+        <v>55.77</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>66.81999999999999</v>
+        <v>55.55</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>65.86</v>
+        <v>50.85</v>
       </c>
     </row>
     <row r="34">
@@ -759,7 +759,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>65.56999999999999</v>
+        <v>75.05</v>
       </c>
     </row>
     <row r="35">
@@ -769,7 +769,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>63.57</v>
+        <v>72.34999999999999</v>
       </c>
     </row>
     <row r="36">
@@ -779,17 +779,17 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>63.59</v>
+        <v>57.72</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>65.68000000000001</v>
+        <v>56.56</v>
       </c>
     </row>
     <row r="38">
@@ -799,7 +799,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>66.01000000000001</v>
+        <v>74.65000000000001</v>
       </c>
     </row>
     <row r="39">
@@ -809,17 +809,17 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>65</v>
+        <v>73.42</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>65.14</v>
+        <v>58.27</v>
       </c>
     </row>
     <row r="41">
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>66.31</v>
+        <v>55.92</v>
       </c>
     </row>
     <row r="42">
@@ -839,7 +839,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>65.31</v>
+        <v>74.81</v>
       </c>
     </row>
     <row r="43">
@@ -849,17 +849,17 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>62.17</v>
+        <v>73.76000000000001</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>67.34999999999999</v>
+        <v>58.86</v>
       </c>
     </row>
     <row r="45">
@@ -869,7 +869,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>65.38</v>
+        <v>55.01</v>
       </c>
     </row>
     <row r="46">
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>64.73999999999999</v>
+        <v>74.88</v>
       </c>
     </row>
     <row r="47">
@@ -889,37 +889,37 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>64.67</v>
+        <v>70.29000000000001</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>65.3</v>
+        <v>58.87</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>54.62</v>
+        <v>51.55</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>79.86</v>
+        <v>73.81999999999999</v>
       </c>
     </row>
     <row r="51">
@@ -929,17 +929,17 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>64.77</v>
+        <v>71.73</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>83.22</v>
+        <v>56.44</v>
       </c>
     </row>
     <row r="53">
@@ -949,37 +949,37 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>62.44</v>
+        <v>71.91</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>83.36</v>
+        <v>65.93000000000001</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>62.46</v>
+        <v>58.56</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>84.56999999999999</v>
+        <v>76.73999999999999</v>
       </c>
     </row>
     <row r="57">
@@ -989,37 +989,37 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>62.02</v>
+        <v>62.82</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>82.94</v>
+        <v>58.05</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>64.01000000000001</v>
+        <v>56.77</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>81.34999999999999</v>
+        <v>50.07</v>
       </c>
     </row>
     <row r="61">
@@ -1029,37 +1029,37 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>63.9</v>
+        <v>84.37</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>76.28</v>
+        <v>59.68</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>65.41</v>
+        <v>55.49</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>51.99</v>
+        <v>51.67</v>
       </c>
     </row>
     <row r="65">
@@ -1069,27 +1069,27 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>63.63</v>
+        <v>87.08</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>57.18</v>
+        <v>57.49</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>76.41</v>
+        <v>57.01</v>
       </c>
     </row>
     <row r="68">
@@ -1099,17 +1099,17 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>61.9</v>
+        <v>84.40000000000001</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>79.43000000000001</v>
+        <v>61.19</v>
       </c>
     </row>
     <row r="70">
@@ -1119,37 +1119,37 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>63.66</v>
+        <v>57.24</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>75.95</v>
+        <v>85.37</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>62.7</v>
+        <v>64.66</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>75.48</v>
+        <v>56.37</v>
       </c>
     </row>
     <row r="74">
@@ -1159,37 +1159,37 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>62.11</v>
+        <v>50.5</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>67.12</v>
+        <v>84.97</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>62.91</v>
+        <v>69.26000000000001</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>76.44</v>
+        <v>55.75</v>
       </c>
     </row>
     <row r="78">
@@ -1199,67 +1199,67 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>64.48</v>
+        <v>84.25</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>50.24</v>
+        <v>68.77</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>81.72</v>
+        <v>57.69</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Bench</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>65.06999999999999</v>
+        <v>51.09</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>82.59999999999999</v>
+        <v>74.43000000000001</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>62.89</v>
+        <v>70.18000000000001</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>80.23999999999999</v>
+        <v>58.72</v>
       </c>
     </row>
     <row r="85">
@@ -1269,37 +1269,37 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>63.54</v>
+        <v>51.91</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Bench</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>63.83</v>
+        <v>50.82</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>62.87</v>
+        <v>70.23999999999999</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>71.40000000000001</v>
+        <v>60.56</v>
       </c>
     </row>
     <row r="89">
@@ -1309,107 +1309,107 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>65.3</v>
+        <v>58.62</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>50.06</v>
+        <v>56.49</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>71.01000000000001</v>
+        <v>53.97</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>64.90000000000001</v>
+        <v>53.35</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Traffic light</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>51.27</v>
+        <v>51.87</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>70.83</v>
+        <v>78.88</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>65.52</v>
+        <v>60.19</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>57.45</v>
+        <v>57.2</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>83.34999999999999</v>
+        <v>56.32</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>64.3</v>
+        <v>51.29</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Traffic light</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>83.56</v>
+        <v>50.81</v>
       </c>
     </row>
     <row r="100">
@@ -1419,37 +1419,37 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>62.74</v>
+        <v>50.19</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>79.98</v>
+        <v>76.06</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>66.04000000000001</v>
+        <v>63.7</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>73.48999999999999</v>
+        <v>60.92</v>
       </c>
     </row>
     <row r="104">
@@ -1459,17 +1459,17 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>66.25</v>
+        <v>56.07</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>75.51000000000001</v>
+        <v>51.18</v>
       </c>
     </row>
     <row r="106">
@@ -1479,47 +1479,47 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>61.28</v>
+        <v>76.29000000000001</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>78.7</v>
+        <v>70.64</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>63.83</v>
+        <v>67.48999999999999</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>53.1</v>
+        <v>56.36</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>79.17</v>
+        <v>75.90000000000001</v>
       </c>
     </row>
     <row r="111">
@@ -1529,27 +1529,27 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>63.09</v>
+        <v>75.19</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>54.56</v>
+        <v>63.86</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>78.41</v>
+        <v>60.25</v>
       </c>
     </row>
     <row r="114">
@@ -1559,57 +1559,57 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>64.05</v>
+        <v>54.05</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>52.69</v>
+        <v>72.37</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>77.02</v>
+        <v>72.18000000000001</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>63.28</v>
+        <v>60.38</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>57.96</v>
+        <v>60.17</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>76.77</v>
+        <v>54.67</v>
       </c>
     </row>
     <row r="120">
@@ -1619,17 +1619,17 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>61.78</v>
+        <v>61.81</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>72.88</v>
+        <v>61.24</v>
       </c>
     </row>
     <row r="122">
@@ -1639,17 +1639,17 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>62.37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>79.22</v>
+        <v>60.44</v>
       </c>
     </row>
     <row r="124">
@@ -1659,57 +1659,57 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>64.89</v>
+        <v>59.77</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>50.19</v>
+        <v>58.47</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>77.11</v>
+        <v>58.31</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>63.92</v>
+        <v>56.11</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>52.62</v>
+        <v>55.28</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>82.69</v>
+        <v>52.74</v>
       </c>
     </row>
     <row r="130">
@@ -1719,57 +1719,57 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>61.46</v>
+        <v>68.05</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>83.29000000000001</v>
+        <v>62.32</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>63.3</v>
+        <v>61.41</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>72.56999999999999</v>
+        <v>59.63</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>63.31</v>
+        <v>58.53</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>77.29000000000001</v>
+        <v>58.08</v>
       </c>
     </row>
     <row r="136">
@@ -1779,157 +1779,157 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>63.76</v>
+        <v>55.83</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>77.48999999999999</v>
+        <v>55.43</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>64.22</v>
+        <v>54.91</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>68.7</v>
+        <v>76.81999999999999</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>66.8</v>
+        <v>66.33</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>69.20999999999999</v>
+        <v>58.54</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>66.09</v>
+        <v>56.79</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>70.37</v>
+        <v>56.65</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>65.90000000000001</v>
+        <v>56.57</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>72.54000000000001</v>
+        <v>56.26</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>63.16</v>
+        <v>55.57</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>70.76000000000001</v>
+        <v>53.12</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>63.3</v>
+        <v>52.56</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>75.36</v>
+        <v>76.68000000000001</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>62.02</v>
+        <v>66.09</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>71.81</v>
+        <v>65.23999999999999</v>
       </c>
     </row>
     <row r="152">
@@ -1939,17 +1939,17 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>63.1</v>
+        <v>59.14</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>71.28</v>
+        <v>54.57</v>
       </c>
     </row>
     <row r="154">
@@ -1959,37 +1959,37 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>63.52</v>
+        <v>54.01</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Traffic light</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>75.22</v>
+        <v>52.74</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>63.29</v>
+        <v>73.65000000000001</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>74.90000000000001</v>
+        <v>70.52</v>
       </c>
     </row>
     <row r="158">
@@ -1999,17 +1999,17 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>61.3</v>
+        <v>63.66</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>76.08</v>
+        <v>54.37</v>
       </c>
     </row>
     <row r="160">
@@ -2019,17 +2019,17 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>61.87</v>
+        <v>54.26</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Traffic light</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>81</v>
+        <v>52.35</v>
       </c>
     </row>
     <row r="162">
@@ -2039,17 +2039,17 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>61.72</v>
+        <v>78.22</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>84.63</v>
+        <v>77.23999999999999</v>
       </c>
     </row>
     <row r="164">
@@ -2059,37 +2059,37 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>62.4</v>
+        <v>65.61</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>83.27</v>
+        <v>56.26</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>64.27</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Traffic light</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>84.22</v>
+        <v>51.52</v>
       </c>
     </row>
     <row r="168">
@@ -2099,17 +2099,17 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>65.09999999999999</v>
+        <v>82.20999999999999</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>81.91</v>
+        <v>79.88</v>
       </c>
     </row>
     <row r="170">
@@ -2119,47 +2119,47 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>63.46</v>
+        <v>63.23</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>50.99</v>
+        <v>58.02</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>80.59</v>
+        <v>52.92</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Traffic light</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>62.3</v>
+        <v>50.22</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>74.23999999999999</v>
+        <v>84.84</v>
       </c>
     </row>
     <row r="175">
@@ -2169,17 +2169,17 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>62.01</v>
+        <v>81.63</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B176" t="n">
-        <v>70.42</v>
+        <v>57.51</v>
       </c>
     </row>
     <row r="177">
@@ -2189,37 +2189,37 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>59.67</v>
+        <v>56.2</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Traffic light</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>66.2</v>
+        <v>50.51</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>60.05</v>
+        <v>80.59</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B180" t="n">
-        <v>74.84</v>
+        <v>79.41</v>
       </c>
     </row>
     <row r="181">
@@ -2229,27 +2229,27 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>60.06</v>
+        <v>57.58</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Traffic light</t>
         </is>
       </c>
       <c r="B182" t="n">
-        <v>53.84</v>
+        <v>52.17</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>73.79000000000001</v>
+        <v>81.53</v>
       </c>
     </row>
     <row r="184">
@@ -2259,7 +2259,7 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>58.88</v>
+        <v>64.75</v>
       </c>
     </row>
     <row r="185">
@@ -2269,27 +2269,27 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>50.73</v>
+        <v>54.63</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Traffic light</t>
         </is>
       </c>
       <c r="B186" t="n">
-        <v>70.73999999999999</v>
+        <v>50.37</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B187" t="n">
-        <v>59.24</v>
+        <v>81.75</v>
       </c>
     </row>
     <row r="188">
@@ -2299,27 +2299,27 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>52.71</v>
+        <v>67.98999999999999</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B189" t="n">
-        <v>69.66</v>
+        <v>54.53</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B190" t="n">
-        <v>57.84</v>
+        <v>80.48</v>
       </c>
     </row>
     <row r="191">
@@ -2329,27 +2329,27 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>56.13</v>
+        <v>68.31999999999999</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Person</t>
         </is>
       </c>
       <c r="B192" t="n">
-        <v>62.24</v>
+        <v>54.69</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B193" t="n">
-        <v>60.32</v>
+        <v>82.34999999999999</v>
       </c>
     </row>
     <row r="194">
@@ -2359,7 +2359,7 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>53.71</v>
+        <v>65.03</v>
       </c>
     </row>
     <row r="195">
@@ -2369,17 +2369,17 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>62.63</v>
+        <v>54.29</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Cell phone</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B196" t="n">
-        <v>50.8</v>
+        <v>77.09</v>
       </c>
     </row>
     <row r="197">
@@ -2389,7 +2389,7 @@
         </is>
       </c>
       <c r="B197" t="n">
-        <v>64.94</v>
+        <v>61.55</v>
       </c>
     </row>
     <row r="198">
@@ -2399,27 +2399,27 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>63.98</v>
+        <v>52.49</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Person</t>
+          <t>Traffic light</t>
         </is>
       </c>
       <c r="B199" t="n">
-        <v>62.86</v>
+        <v>50.38</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Bottle</t>
+          <t>Car</t>
         </is>
       </c>
       <c r="B200" t="n">
-        <v>53.53</v>
+        <v>81.72</v>
       </c>
     </row>
     <row r="201">
@@ -2429,7 +2429,2347 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>64.69</v>
+        <v>55.86</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>53.02</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>51.94</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>79.33</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>53.74</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>79.18000000000001</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>54.1</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>50.08</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>79.98</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>52.9</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>83.66</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>68.69</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>56.58</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>54.41</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>53.84</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>81.54000000000001</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>70.78</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>62.82</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>57.35</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>52.63</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>82.73</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>71.06</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>59.39</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>58.1</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>56.84</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>54.16</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>50.76</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>78.56</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B230" t="n">
+        <v>73.08</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>60.13</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>59.57</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>53.69</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>51.41</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>78.44</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>70.89</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>60.78</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>60.71</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>54.7</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>54.15</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>80.23</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B243" t="n">
+        <v>71.29000000000001</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B244" t="n">
+        <v>65.56999999999999</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>55.45</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>54.22</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>53.7</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>80.59</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>69.65000000000001</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>64.78</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>59.11</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>58.86</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>55.58</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>51.21</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>80.39</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>67.92</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>64.3</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>62.85</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>57.89</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>57.31</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>56.01</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>52.7</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>78.84999999999999</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>69.2</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>68.04000000000001</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>58.39</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>57.05</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>56.55</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>52.27</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>78.26000000000001</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>68.7</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>56.53</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>56.27</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>55.69</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>55.12</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>80.17</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>64.56999999999999</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>62.27</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>57.15</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>56.23</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>54.19</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>53.99</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>84.56999999999999</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>63.95</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>61.73</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>59.54</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>56.49</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>56.23</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>52.32</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>84.59</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>63.91</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>63.15</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>61.32</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>60.66</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>57.56</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>55.76</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>51.15</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>81.12</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>63.92</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>61.15</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>61.07</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>59.51</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B306" t="n">
+        <v>56.49</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B307" t="n">
+        <v>54.53</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B308" t="n">
+        <v>80.73</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B309" t="n">
+        <v>66.12</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B310" t="n">
+        <v>62.64</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B311" t="n">
+        <v>57.85</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B312" t="n">
+        <v>55.99</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B313" t="n">
+        <v>55.45</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B314" t="n">
+        <v>55.17</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B315" t="n">
+        <v>82.23999999999999</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B316" t="n">
+        <v>68.48999999999999</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B317" t="n">
+        <v>68.28</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B318" t="n">
+        <v>60.17</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B319" t="n">
+        <v>59.66</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B320" t="n">
+        <v>55.46</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B321" t="n">
+        <v>54.58</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B322" t="n">
+        <v>81.54000000000001</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B323" t="n">
+        <v>68.59999999999999</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B324" t="n">
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B325" t="n">
+        <v>62.13</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B326" t="n">
+        <v>60.16</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B327" t="n">
+        <v>55.74</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B328" t="n">
+        <v>53.08</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B329" t="n">
+        <v>82.73999999999999</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B330" t="n">
+        <v>69.93000000000001</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B331" t="n">
+        <v>68.63</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B332" t="n">
+        <v>60.22</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B333" t="n">
+        <v>56.94</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B334" t="n">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B335" t="n">
+        <v>52.21</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B336" t="n">
+        <v>50.78</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B337" t="n">
+        <v>50.37</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B338" t="n">
+        <v>82.92</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B339" t="n">
+        <v>71.70999999999999</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B340" t="n">
+        <v>71.29000000000001</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B341" t="n">
+        <v>59.96</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B342" t="n">
+        <v>56.41</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B343" t="n">
+        <v>55.22</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B344" t="n">
+        <v>53.42</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B345" t="n">
+        <v>52.14</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B346" t="n">
+        <v>80.48999999999999</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B347" t="n">
+        <v>72.17</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B348" t="n">
+        <v>70.95</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B349" t="n">
+        <v>62.92</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B350" t="n">
+        <v>58.66</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B351" t="n">
+        <v>56.39</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B352" t="n">
+        <v>55.01</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B353" t="n">
+        <v>77.61</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B354" t="n">
+        <v>67.04000000000001</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B355" t="n">
+        <v>65.77</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B356" t="n">
+        <v>64.75</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B357" t="n">
+        <v>56.53</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B358" t="n">
+        <v>56.29</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B359" t="n">
+        <v>55.64</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B360" t="n">
+        <v>51.37</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B361" t="n">
+        <v>71.12</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B362" t="n">
+        <v>69.3</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B363" t="n">
+        <v>66.23</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B364" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B365" t="n">
+        <v>58.14</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B366" t="n">
+        <v>56.22</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B367" t="n">
+        <v>53.42</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>Traffic light</t>
+        </is>
+      </c>
+      <c r="B368" t="n">
+        <v>50.12</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B369" t="n">
+        <v>72.81999999999999</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B370" t="n">
+        <v>69.45999999999999</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B371" t="n">
+        <v>68.65000000000001</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B372" t="n">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B373" t="n">
+        <v>57.25</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B374" t="n">
+        <v>56.88</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B375" t="n">
+        <v>55.16</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B376" t="n">
+        <v>70.14</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B377" t="n">
+        <v>70.12</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B378" t="n">
+        <v>64.01000000000001</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B379" t="n">
+        <v>59.72</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B380" t="n">
+        <v>56.96</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B381" t="n">
+        <v>56.88</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B382" t="n">
+        <v>54.32</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B383" t="n">
+        <v>50.49</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B384" t="n">
+        <v>50.13</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B385" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B386" t="n">
+        <v>68.48999999999999</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B387" t="n">
+        <v>63.19</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B388" t="n">
+        <v>57.54</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B389" t="n">
+        <v>56.12</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B390" t="n">
+        <v>55.89</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B391" t="n">
+        <v>51.08</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B392" t="n">
+        <v>51.06</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B393" t="n">
+        <v>50.4</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B394" t="n">
+        <v>71.62</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B395" t="n">
+        <v>67.69</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B396" t="n">
+        <v>57.16</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B397" t="n">
+        <v>55.67</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B398" t="n">
+        <v>53.43</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B399" t="n">
+        <v>69.92</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B400" t="n">
+        <v>68.67</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B401" t="n">
+        <v>56.33</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B402" t="n">
+        <v>54.78</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B403" t="n">
+        <v>53.39</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B404" t="n">
+        <v>50.49</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B405" t="n">
+        <v>70.34</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B406" t="n">
+        <v>68.31</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B407" t="n">
+        <v>58.73</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B408" t="n">
+        <v>56.02</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B409" t="n">
+        <v>55.49</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B410" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B411" t="n">
+        <v>71.29000000000001</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B412" t="n">
+        <v>71.26000000000001</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B413" t="n">
+        <v>59.34</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B414" t="n">
+        <v>56.6</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B415" t="n">
+        <v>56.15</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B416" t="n">
+        <v>55.01</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B417" t="n">
+        <v>53.27</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B418" t="n">
+        <v>73.25</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B419" t="n">
+        <v>69.86</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B420" t="n">
+        <v>58.44</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B421" t="n">
+        <v>56.87</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B422" t="n">
+        <v>55.27</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B423" t="n">
+        <v>52.98</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B424" t="n">
+        <v>74.59</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B425" t="n">
+        <v>66.47</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B426" t="n">
+        <v>56.48</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B427" t="n">
+        <v>55.46</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B428" t="n">
+        <v>52.53</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B429" t="n">
+        <v>51.28</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B430" t="n">
+        <v>72.77</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B431" t="n">
+        <v>69.28</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B432" t="n">
+        <v>57.36</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B433" t="n">
+        <v>56.74</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B434" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>Person</t>
+        </is>
+      </c>
+      <c r="B435" t="n">
+        <v>53.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>